<commit_message>
se soluciona error al exportar archivo html de benchmark
</commit_message>
<xml_diff>
--- a/Data/2023/1. Enero 2023/Registro_de_operaciones_Roboforex_Enero2023.xlsx
+++ b/Data/2023/1. Enero 2023/Registro_de_operaciones_Roboforex_Enero2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\QuantCo_Streamlit\Data\2023\1. Enero 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455F54D6-35BC-4869-BDF4-57D2393E3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40C2629-AF2F-4A1A-8DC9-45BDD1CC22D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="160">
   <si>
     <t>Size</t>
   </si>
@@ -520,8 +520,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -560,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -568,6 +569,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,13 +886,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A156" sqref="A2:A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.09765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -918,7 +920,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
@@ -942,7 +944,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -967,7 +969,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -992,7 +994,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -1017,7 +1019,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -1042,7 +1044,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
@@ -1067,7 +1069,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B8">
@@ -1092,7 +1094,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B9">
@@ -1117,7 +1119,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B10">
@@ -1142,7 +1144,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -1167,7 +1169,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B12">
@@ -1192,7 +1194,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B13">
@@ -1217,7 +1219,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B14">
@@ -1242,7 +1244,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B15">
@@ -1267,7 +1269,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B16">
@@ -1292,7 +1294,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B17">
@@ -1317,7 +1319,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B18">
@@ -1342,7 +1344,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B19">
@@ -1367,7 +1369,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B20">
@@ -1392,7 +1394,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B21">
@@ -1417,7 +1419,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B22">
@@ -1442,7 +1444,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B23">
@@ -1467,7 +1469,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B24">
@@ -1492,7 +1494,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B25">
@@ -1517,7 +1519,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B26">
@@ -1542,7 +1544,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B27">
@@ -1567,7 +1569,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B28">
@@ -1592,7 +1594,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B29">
@@ -1617,7 +1619,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B30">
@@ -1642,7 +1644,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B31">
@@ -1667,7 +1669,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B32">
@@ -1692,7 +1694,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B33">
@@ -1717,7 +1719,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B34">
@@ -1742,7 +1744,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B35">
@@ -1767,7 +1769,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B36">
@@ -1792,7 +1794,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B37">
@@ -1817,7 +1819,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B38">
@@ -1842,7 +1844,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B39">
@@ -1867,7 +1869,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B40">
@@ -1892,7 +1894,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B41">
@@ -1917,7 +1919,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B42">
@@ -1942,7 +1944,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B43">
@@ -1967,7 +1969,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B44">
@@ -1992,7 +1994,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B45">
@@ -2017,7 +2019,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B46">
@@ -2042,7 +2044,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B47">
@@ -2067,7 +2069,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B48">
@@ -2092,7 +2094,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B49">
@@ -2117,7 +2119,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B50">
@@ -2142,7 +2144,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B51">
@@ -2167,7 +2169,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B52">
@@ -2192,7 +2194,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B53">
@@ -2217,7 +2219,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B54">
@@ -2242,7 +2244,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B55">
@@ -2267,7 +2269,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B56">
@@ -2292,7 +2294,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B57">
@@ -2317,7 +2319,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B58">
@@ -2342,7 +2344,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B59">
@@ -2367,7 +2369,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B60">
@@ -2392,7 +2394,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B61">
@@ -2417,7 +2419,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B62">
@@ -2442,7 +2444,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B63">
@@ -2467,7 +2469,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B64">
@@ -2492,7 +2494,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B65">
@@ -2517,7 +2519,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B66">
@@ -2542,7 +2544,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B67">
@@ -2567,7 +2569,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B68">
@@ -2592,7 +2594,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B69">
@@ -2617,7 +2619,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B70">
@@ -2642,7 +2644,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B71">
@@ -2667,7 +2669,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B72">
@@ -2692,7 +2694,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B73">
@@ -2717,7 +2719,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B74">
@@ -2742,7 +2744,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B75">
@@ -2767,7 +2769,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B76">
@@ -2792,7 +2794,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B77">
@@ -2817,7 +2819,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B78">
@@ -2842,7 +2844,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B79">
@@ -2867,7 +2869,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B80">
@@ -2892,7 +2894,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B81">
@@ -2917,7 +2919,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B82">
@@ -2942,7 +2944,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B83">
@@ -2967,7 +2969,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B84">
@@ -2992,7 +2994,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B85">
@@ -3017,7 +3019,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B86">
@@ -3042,7 +3044,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B87">
@@ -3067,7 +3069,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B88">
@@ -3092,7 +3094,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B89">
@@ -3117,7 +3119,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B90">
@@ -3142,7 +3144,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+      <c r="A91" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B91">
@@ -3167,7 +3169,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B92">
@@ -3192,7 +3194,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B93">
@@ -3217,7 +3219,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
+      <c r="A94" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B94">
@@ -3242,7 +3244,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+      <c r="A95" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B95">
@@ -3267,7 +3269,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B96">
@@ -3292,7 +3294,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B97">
@@ -3317,7 +3319,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B98">
@@ -3342,7 +3344,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B99">
@@ -3367,7 +3369,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B100">
@@ -3392,7 +3394,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B101">
@@ -3417,7 +3419,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B102">
@@ -3442,7 +3444,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
+      <c r="A103" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B103">
@@ -3467,7 +3469,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B104">
@@ -3492,7 +3494,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B105">
@@ -3517,7 +3519,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
+      <c r="A106" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B106">
@@ -3542,7 +3544,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B107">
@@ -3567,7 +3569,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B108">
@@ -3592,7 +3594,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="7" t="s">
         <v>110</v>
       </c>
       <c r="B109">
@@ -3617,7 +3619,7 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
+      <c r="A110" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B110">
@@ -3642,7 +3644,7 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
+      <c r="A111" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B111">
@@ -3667,7 +3669,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="6" t="s">
+      <c r="A112" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B112">
@@ -3692,7 +3694,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="6" t="s">
+      <c r="A113" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B113">
@@ -3717,7 +3719,7 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B114">
@@ -3742,7 +3744,7 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
+      <c r="A115" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B115">
@@ -3767,7 +3769,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
+      <c r="A116" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B116">
@@ -3792,7 +3794,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="6" t="s">
+      <c r="A117" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B117">
@@ -3817,7 +3819,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B118">
@@ -3842,7 +3844,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B119">
@@ -3867,7 +3869,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B120">
@@ -3892,7 +3894,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="6" t="s">
+      <c r="A121" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B121">
@@ -3917,7 +3919,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="6" t="s">
+      <c r="A122" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B122">
@@ -3942,7 +3944,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="6" t="s">
+      <c r="A123" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B123">
@@ -3967,7 +3969,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B124">
@@ -3992,7 +3994,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B125">
@@ -4017,7 +4019,7 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B126">
@@ -4042,7 +4044,7 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="6" t="s">
+      <c r="A127" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B127">
@@ -4067,7 +4069,7 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B128">
@@ -4092,7 +4094,7 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B129">
@@ -4117,7 +4119,7 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="6" t="s">
+      <c r="A130" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B130">
@@ -4142,7 +4144,7 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B131">
@@ -4167,7 +4169,7 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B132">
@@ -4192,7 +4194,7 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B133">
@@ -4217,7 +4219,7 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="7" t="s">
         <v>135</v>
       </c>
       <c r="B134">
@@ -4242,7 +4244,7 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B135">
@@ -4267,7 +4269,7 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B136">
@@ -4292,7 +4294,7 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B137">
@@ -4317,7 +4319,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B138">
@@ -4342,7 +4344,7 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="6" t="s">
+      <c r="A139" s="7" t="s">
         <v>140</v>
       </c>
       <c r="B139">
@@ -4367,7 +4369,7 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B140">
@@ -4392,7 +4394,7 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B141">
@@ -4417,7 +4419,7 @@
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B142">
@@ -4442,7 +4444,7 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B143">
@@ -4467,7 +4469,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B144">
@@ -4492,7 +4494,7 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B145">
@@ -4517,7 +4519,7 @@
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B146">
@@ -4542,7 +4544,7 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B147">
@@ -4567,7 +4569,7 @@
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B148">
@@ -4592,7 +4594,7 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="7" t="s">
         <v>150</v>
       </c>
       <c r="B149">
@@ -4617,7 +4619,7 @@
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B150">
@@ -4642,7 +4644,7 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B151">
@@ -4667,7 +4669,7 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="7" t="s">
         <v>153</v>
       </c>
       <c r="B152">
@@ -4692,7 +4694,7 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B153">
@@ -4717,7 +4719,7 @@
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B154">
@@ -4742,7 +4744,7 @@
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="6" t="s">
+      <c r="A155" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B155">
@@ -4767,8 +4769,8 @@
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="6">
-        <v>44957.490972222222</v>
+      <c r="A156" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="B156">
         <v>0.02</v>
@@ -4801,5 +4803,6 @@
   <autoFilter ref="A1:G156" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>